<commit_message>
refreshed metadata file and removed extra file
</commit_message>
<xml_diff>
--- a/test_files/test_metadata.xlsx
+++ b/test_files/test_metadata.xlsx
@@ -1,40 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunkerly\Documents\GitHub\pyWeatherQAQC\test_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC61A4CA-BAD2-4663-934A-0125FDAB9076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>station_name</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>elev_m</t>
+  </si>
+  <si>
+    <t>record_start</t>
+  </si>
+  <si>
+    <t>record_end</t>
+  </si>
+  <si>
+    <t>anemom_height_m</t>
+  </si>
+  <si>
+    <t>input_path</t>
+  </si>
+  <si>
+    <t>output_path</t>
+  </si>
+  <si>
+    <t>run_count</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>test_files/test_data.csv</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD" numFmtId="165"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,27 +105,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,132 +430,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>station_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>latitude</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>longitude</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>elev_m</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>record_start</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>record_end</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>anemom_height_m</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>input_path</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>output_path</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>run_count</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>6</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>38.535794</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>38.535794000000003</v>
+      </c>
+      <c r="E2">
         <v>-121.776385</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>18.288</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>34336</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>43465</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>test_files/test_data.csv</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>test_files/correction_files/6_output.xlsx</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
renamed files in move towards pypi package, streamlined script performance
Script is no longer run twice per file in a manner toggled by 'correction_mode' in the config file, processing speed is improved by removing redundant calcs
</commit_message>
<xml_diff>
--- a/test_files/test_metadata.xlsx
+++ b/test_files/test_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunkerly\Documents\GitHub\pyWeatherQAQC\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC61A4CA-BAD2-4663-934A-0125FDAB9076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC61D707-9A40-4CC5-91D8-79C9BEAC9BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>output_path</t>
   </si>
   <si>
-    <t>run_count</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>test_files/test_data.csv</t>
+  </si>
+  <si>
+    <t>processed</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,10 +489,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>38.535794000000003</v>
@@ -520,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L2">
         <v>0</v>

</xml_diff>

<commit_message>
Overhauled docs, updated environment.yml, improved wording on function documentation, renamed plotting_functions
also re-added second testing dataset
</commit_message>
<xml_diff>
--- a/test_files/test_metadata.xlsx
+++ b/test_files/test_metadata.xlsx
@@ -1,96 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunkerly\Documents\GitHub\pyWeatherQAQC\test_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC61D707-9A40-4CC5-91D8-79C9BEAC9BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>station_name</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>elev_m</t>
-  </si>
-  <si>
-    <t>record_start</t>
-  </si>
-  <si>
-    <t>record_end</t>
-  </si>
-  <si>
-    <t>anemom_height_m</t>
-  </si>
-  <si>
-    <t>input_path</t>
-  </si>
-  <si>
-    <t>output_path</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Davis</t>
-  </si>
-  <si>
-    <t>test_files/test_data.csv</t>
-  </si>
-  <si>
-    <t>processed</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -105,44 +51,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -430,100 +427,167 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>station_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>elev_m</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>record_start</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>record_end</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>anemom_height_m</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>input_path</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>output_path</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Davis</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>38.535794</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-121.776385</v>
+      </c>
+      <c r="F2" t="n">
+        <v>18.288</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>34335</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>43465</v>
+      </c>
+      <c r="I2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>test_files/test_data.csv</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>test_files/correction_files/output_data/6_output.xlsx</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Durham</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>39.60864</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-121.824</v>
+      </c>
+      <c r="F3" t="n">
+        <v>39.624</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>42370</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>45012</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>test_files/test_data_2.csv</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>test_files/correction_files/output_data/12_output.xlsx</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>38.535794000000003</v>
-      </c>
-      <c r="E2">
-        <v>-121.776385</v>
-      </c>
-      <c r="F2">
-        <v>18.288</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>